<commit_message>
put option -y in install batch
</commit_message>
<xml_diff>
--- a/calib/Calibration_1.xlsx
+++ b/calib/Calibration_1.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="45" windowWidth="12450" windowHeight="10620" activeTab="2"/>
+    <workbookView xWindow="-15" yWindow="45" windowWidth="12450" windowHeight="10620" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="turbidity_ODL_#40" sheetId="1" r:id="rId1"/>
     <sheet name="turbidity_soilTest_#60" sheetId="4" r:id="rId2"/>
     <sheet name="turbidity_soilTest_#60 (ODL)" sheetId="5" r:id="rId3"/>
     <sheet name="pressure" sheetId="2" r:id="rId4"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
+    <sheet name="datasheet" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'turbidity_ODL_#40'!#REF!</definedName>
@@ -19,7 +19,6 @@
     <definedName name="_xlnm.Print_Area" localSheetId="2">'turbidity_soilTest_#60 (ODL)'!#REF!</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -218,7 +217,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-sujidade parasita</t>
+"zer0"</t>
         </r>
       </text>
     </comment>
@@ -243,6 +242,7 @@
           </rPr>
           <t xml:space="preserve">
 tap water
+com piklete a rodar
 </t>
         </r>
       </text>
@@ -252,7 +252,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
   <si>
     <t>psi</t>
   </si>
@@ -299,22 +299,134 @@
     <t>water volume used:</t>
   </si>
   <si>
-    <t>ln</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>Tb=</t>
-  </si>
-  <si>
-    <t>Tb</t>
-  </si>
-  <si>
     <t>analog#</t>
   </si>
   <si>
     <t>turbidity</t>
+  </si>
+  <si>
+    <t>peso total=</t>
+  </si>
+  <si>
+    <t>x2</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>www.amphenol-sensors.com</t>
+  </si>
+  <si>
+    <t>TSW-10</t>
+  </si>
+  <si>
+    <t>Turbidity Sensor</t>
+  </si>
+  <si>
+    <r>
+      <t>1E-11x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 2E-07x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - 0.0016x + 4.7176</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>-1E-10x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + 8E-07x</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - 0.0019x + 3.6454</t>
+    </r>
+  </si>
+  <si>
+    <t>x3</t>
+  </si>
+  <si>
+    <t>NTU</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>https://pt.mouser.com/datasheet/2/18/AAS-920-479B-Thermometrics-TSW-10-052214-web-1315877.pdf</t>
   </si>
 </sst>
 </file>
@@ -324,7 +436,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -419,6 +531,27 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -585,7 +718,7 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -670,6 +803,13 @@
     </xf>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -909,11 +1049,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="42941440"/>
-        <c:axId val="42947712"/>
+        <c:axId val="49790976"/>
+        <c:axId val="49792896"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="42941440"/>
+        <c:axId val="49790976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="32768"/>
@@ -951,12 +1091,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42947712"/>
+        <c:crossAx val="49792896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="42947712"/>
+        <c:axId val="49792896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1004,7 +1144,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42941440"/>
+        <c:crossAx val="49790976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1491,11 +1631,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="42956672"/>
-        <c:axId val="42836736"/>
+        <c:axId val="49851776"/>
+        <c:axId val="49870336"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="42956672"/>
+        <c:axId val="49851776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25000"/>
@@ -1533,12 +1673,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42836736"/>
+        <c:crossAx val="49870336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="42836736"/>
+        <c:axId val="49870336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1"/>
@@ -1586,7 +1726,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42956672"/>
+        <c:crossAx val="49851776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1638,19 +1778,19 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="1100"/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="1100"/>
               <a:t>Turbidimeter </a:t>
             </a:r>
           </a:p>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="1100"/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="1100"/>
               <a:t>Calibration</a:t>
             </a:r>
           </a:p>
@@ -1660,8 +1800,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.35307830168057441"/>
-          <c:y val="3.3534872636798184E-2"/>
+          <c:x val="0.44610680654982737"/>
+          <c:y val="0"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1685,20 +1825,19 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>Test_soil</c:v>
-          </c:tx>
           <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
-            </a:ln>
+            <a:ln w="12700"/>
           </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="2"/>
+          </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'turbidity_soilTest_#60 (ODL)'!$C$6:$C$32</c:f>
+              <c:f>'turbidity_soilTest_#60 (ODL)'!$C$6:$C$51</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="0">
                   <c:v>29617.555555555555</c:v>
                 </c:pt>
@@ -1779,16 +1918,73 @@
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>20709.888888888891</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>19952.666666666668</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>19187.875</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>18408.714285714286</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>17835.25</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>16783.25</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>15633.428571428571</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>13957.111111111111</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>12716.125</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>10903.285714285714</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9472.8333333333339</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>8024.1428571428569</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>6389.1428571428569</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>5229.7142857142853</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4013.8571428571427</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>3169.5714285714284</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2283.4285714285716</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1671.4285714285713</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1153.8</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>777.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'turbidity_soilTest_#60 (ODL)'!$D$6:$D$32</c:f>
+              <c:f>'turbidity_soilTest_#60 (ODL)'!$D$6:$D$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1870,195 +2066,62 @@
                 <c:pt idx="26">
                   <c:v>2.4</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:spPr>
-            <a:ln w="28575">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'turbidity_soilTest_#60 (ODL)'!$C$6:$C$32</c:f>
-              <c:numCache>
-                <c:formatCode>0</c:formatCode>
-                <c:ptCount val="27"/>
-                <c:pt idx="0">
-                  <c:v>29617.555555555555</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>29586.375</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>29429.625</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>29364.111111111109</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>29211</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>29102.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>28956.777777777777</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>28890</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>28513.666666666668</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>28282.5</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>28124.666666666668</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>27914</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>27665.333333333332</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>27385.333333333332</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>27176.777777777777</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>26767.7</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>26015</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>25780.3</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>25482.5</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>24898.1</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>24496</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>23781.5</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>23270.7</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>22913.4</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>22414.444444444445</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>21633.25</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>20709.888888888891</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'turbidity_soilTest_#60 (ODL)'!$D$6:$D$32</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.5000000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.05</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7.4999999999999997E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.125</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.15000000000000002</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.17499999999999999</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.23749999999999999</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.3</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.36249999999999999</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.42499999999999993</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.48749999999999993</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.54999999999999993</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.61249999999999993</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.67499999999999982</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.86250000000000004</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.98749999999999982</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1.0999999999999999</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1.2249999999999999</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1.3499999999999996</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1.5249999999999997</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1.6499999999999997</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1.8</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1.9</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>2.15</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>2.4</c:v>
+                <c:pt idx="27">
+                  <c:v>2.65</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.9000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.1500000000000004</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3.9000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4.5500000000000007</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5.3</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>6.0750000000000002</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>7.0750000000000002</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>8.3249999999999993</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>9.8249999999999993</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>11.574999999999999</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>13.574999999999999</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>15.824999999999999</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>18.324999999999999</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>22.074999999999999</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>27.074999999999999</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>34.575000000000003</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>47.075000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2073,13 +2136,14 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="42901504"/>
-        <c:axId val="42903424"/>
+        <c:axId val="50662400"/>
+        <c:axId val="50676864"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="42901504"/>
+        <c:axId val="50662400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="100"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -2113,12 +2177,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42903424"/>
+        <c:crossAx val="50676864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="42903424"/>
+        <c:axId val="50676864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2146,7 +2210,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>turbidity (grams/)</a:t>
+                  <a:t>turbidity (grams/liter)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2165,7 +2229,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42901504"/>
+        <c:crossAx val="50662400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2176,14 +2240,289 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.24721625443705905"/>
-          <c:y val="0.62128236560800776"/>
-          <c:w val="0.28419197842827121"/>
-          <c:h val="0.14858556112489693"/>
+          <c:x val="0.57007989507039403"/>
+          <c:y val="0.17694530317043178"/>
+          <c:w val="0.1621783756280252"/>
+          <c:h val="7.5801024661994232E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
     </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.28456933508311461"/>
+                  <c:y val="-0.49985922847177261"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>datasheet!$F$9:$F$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1750</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>datasheet!$G$9:$G$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.38</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.68</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.82</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-6.6248906386701658E-3"/>
+                  <c:y val="3.0577915161135363E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>datasheet!$F$9:$F$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1750</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>datasheet!$H$9:$H$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>3.65</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.85</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.35</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.1800000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.0499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.92</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.81</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="44885120"/>
+        <c:axId val="44879232"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="44885120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="2000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:minorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="44879232"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="500"/>
+        <c:minorUnit val="250"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="44879232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="1.5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="44885120"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="0.25"/>
+      </c:valAx>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -2272,16 +2611,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>486757</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>218866</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>72107</xdr:rowOff>
+      <xdr:rowOff>185216</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>175345</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>169392</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>53789</xdr:rowOff>
+      <xdr:rowOff>166898</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2300,6 +2639,79 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>342550</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>8608</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14611350" y="1257300"/>
+          <a:ext cx="2800000" cy="7342858"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2998,10 +3410,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K32"/>
+  <dimension ref="A2:I32"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F4" sqref="F4:K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3020,7 +3432,7 @@
     <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>14</v>
       </c>
@@ -3031,7 +3443,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>11</v>
       </c>
@@ -3042,29 +3454,13 @@
         <v>7</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="1">
-        <v>-4.3369999999999997</v>
-      </c>
-      <c r="H4" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="1" t="str">
-        <f>"+"</f>
-        <v>+</v>
-      </c>
-      <c r="K4" s="1">
-        <v>44.155000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="11"/>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
         <v>9</v>
       </c>
@@ -3072,14 +3468,14 @@
         <v>13</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="9"/>
     </row>
-    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="15">
         <v>0</v>
       </c>
@@ -3096,14 +3492,10 @@
         <v>0</v>
       </c>
       <c r="E6" s="9"/>
-      <c r="F6" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="22" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>0.1</v>
       </c>
@@ -3120,15 +3512,9 @@
         <v>0.25</v>
       </c>
       <c r="E7" s="8"/>
-      <c r="F7" s="22">
-        <v>27200</v>
-      </c>
-      <c r="G7" s="1">
-        <f>$G$4*LN(F7)+$K$4</f>
-        <v>-0.12998665815609201</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F7" s="22"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>0.1</v>
       </c>
@@ -3145,15 +3531,9 @@
         <v>0.5</v>
       </c>
       <c r="E8" s="8"/>
-      <c r="F8" s="22">
-        <v>1900</v>
-      </c>
-      <c r="G8" s="1">
-        <f>$G$4*LN(F8)+$K$4</f>
-        <v>11.412345050724795</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F8" s="22"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>0.1</v>
       </c>
@@ -3171,7 +3551,7 @@
       </c>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>0.1</v>
       </c>
@@ -3189,7 +3569,7 @@
       </c>
       <c r="E10" s="8"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>0.1</v>
       </c>
@@ -3207,7 +3587,7 @@
       </c>
       <c r="E11" s="8"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>0.2</v>
       </c>
@@ -3225,7 +3605,7 @@
       </c>
       <c r="E12" s="8"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>0.2</v>
       </c>
@@ -3243,7 +3623,7 @@
       </c>
       <c r="E13" s="8"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>0.2</v>
       </c>
@@ -3261,7 +3641,7 @@
       </c>
       <c r="E14" s="8"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>0.2</v>
       </c>
@@ -3279,7 +3659,7 @@
       </c>
       <c r="E15" s="8"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>0.2</v>
       </c>
@@ -3591,10 +3971,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K33"/>
+  <dimension ref="A2:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="160" zoomScaleNormal="160" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3613,7 +3993,7 @@
     <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>14</v>
       </c>
@@ -3627,8 +4007,15 @@
         <f>AVERAGE(29552,29556,29555,29577,29574,29554,29619,29615)</f>
         <v>29575.25</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="1">
+        <f>752-12-214.3-500</f>
+        <v>25.700000000000045</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>11</v>
       </c>
@@ -3639,29 +4026,13 @@
         <v>7</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="1">
-        <v>-4.3369999999999997</v>
-      </c>
-      <c r="H4" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="1" t="str">
-        <f>"+"</f>
-        <v>+</v>
-      </c>
-      <c r="K4" s="1">
-        <v>44.155000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="11"/>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
         <v>9</v>
       </c>
@@ -3669,14 +4040,14 @@
         <v>13</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="9"/>
     </row>
-    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="15">
         <v>0</v>
       </c>
@@ -3693,14 +4064,10 @@
         <v>0</v>
       </c>
       <c r="E6" s="9"/>
-      <c r="F6" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="22" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>0.01</v>
       </c>
@@ -3717,20 +4084,14 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="E7" s="8"/>
-      <c r="F7" s="22">
-        <v>27200</v>
-      </c>
-      <c r="G7" s="1">
-        <f>$G$4*LN(F7)+$K$4</f>
-        <v>-0.12998665815609201</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F7" s="22"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>0.01</v>
       </c>
       <c r="B8" s="1">
-        <f t="shared" ref="B8:B33" si="1">B7+A8</f>
+        <f t="shared" ref="B8:B51" si="1">B7+A8</f>
         <v>0.02</v>
       </c>
       <c r="C8" s="13">
@@ -3742,15 +4103,9 @@
         <v>0.05</v>
       </c>
       <c r="E8" s="8"/>
-      <c r="F8" s="22">
-        <v>1900</v>
-      </c>
-      <c r="G8" s="1">
-        <f>$G$4*LN(F8)+$K$4</f>
-        <v>11.412345050724795</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F8" s="22"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>0.01</v>
       </c>
@@ -3768,7 +4123,7 @@
       </c>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>0.01</v>
       </c>
@@ -3786,7 +4141,7 @@
       </c>
       <c r="E10" s="8"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>0.01</v>
       </c>
@@ -3804,7 +4159,7 @@
       </c>
       <c r="E11" s="8"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>0.01</v>
       </c>
@@ -3822,7 +4177,7 @@
       </c>
       <c r="E12" s="8"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>0.01</v>
       </c>
@@ -3840,7 +4195,7 @@
       </c>
       <c r="E13" s="8"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -3858,7 +4213,7 @@
       </c>
       <c r="E14" s="8"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -3876,7 +4231,7 @@
       </c>
       <c r="E15" s="8"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -4060,7 +4415,7 @@
       <c r="A26" s="19">
         <v>0.05</v>
       </c>
-      <c r="B26" s="20">
+      <c r="B26" s="1">
         <f t="shared" si="1"/>
         <v>0.53999999999999992</v>
       </c>
@@ -4190,6 +4545,318 @@
       <c r="D33" s="1">
         <f t="shared" si="0"/>
         <v>2.65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="B34" s="1">
+        <f t="shared" si="1"/>
+        <v>1.1600000000000001</v>
+      </c>
+      <c r="C34" s="13">
+        <f>AVERAGE(18762,19427,18855,19377,19172,19520,19320,19070)</f>
+        <v>19187.875</v>
+      </c>
+      <c r="D34" s="1">
+        <f t="shared" ref="D34:D36" si="2">B34*1000/400</f>
+        <v>2.9000000000000004</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="B35" s="1">
+        <f t="shared" si="1"/>
+        <v>1.2600000000000002</v>
+      </c>
+      <c r="C35" s="13">
+        <f>AVERAGE(18546,18064,18570,18477,18386,18588,18230)</f>
+        <v>18408.714285714286</v>
+      </c>
+      <c r="D35" s="1">
+        <f t="shared" si="2"/>
+        <v>3.1500000000000004</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="B36" s="1">
+        <f t="shared" si="1"/>
+        <v>1.3600000000000003</v>
+      </c>
+      <c r="C36" s="13">
+        <f>AVERAGE(17359,17994,17874,18089,17948,17790,18201,17427)</f>
+        <v>17835.25</v>
+      </c>
+      <c r="D36" s="1">
+        <f t="shared" si="2"/>
+        <v>3.4000000000000004</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="B37" s="1">
+        <f t="shared" si="1"/>
+        <v>1.5600000000000003</v>
+      </c>
+      <c r="C37" s="13">
+        <f>AVERAGE(16666,16754,17142,17000,16617,16069,16797,17221)</f>
+        <v>16783.25</v>
+      </c>
+      <c r="D37" s="1">
+        <f t="shared" ref="D37" si="3">B37*1000/400</f>
+        <v>3.9000000000000004</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="10">
+        <v>0.26</v>
+      </c>
+      <c r="B38" s="1">
+        <f t="shared" si="1"/>
+        <v>1.8200000000000003</v>
+      </c>
+      <c r="C38" s="13">
+        <f>AVERAGE(15515,15083,15486,15839,15806,15609,16096)</f>
+        <v>15633.428571428571</v>
+      </c>
+      <c r="D38" s="1">
+        <f t="shared" ref="D38" si="4">B38*1000/400</f>
+        <v>4.5500000000000007</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="B39" s="1">
+        <f t="shared" si="1"/>
+        <v>2.12</v>
+      </c>
+      <c r="C39" s="13">
+        <f>AVERAGE(14138,13663,14197,13640,14124,13666,14059,14048,14079)</f>
+        <v>13957.111111111111</v>
+      </c>
+      <c r="D39" s="1">
+        <f t="shared" ref="D39" si="5">B39*1000/400</f>
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="10">
+        <v>0.31</v>
+      </c>
+      <c r="B40" s="1">
+        <f t="shared" si="1"/>
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="C40" s="13">
+        <f>AVERAGE(12774,12888,12846,12820,13100,12616,12090,12595)</f>
+        <v>12716.125</v>
+      </c>
+      <c r="D40" s="1">
+        <f t="shared" ref="D40" si="6">B40*1000/400</f>
+        <v>6.0750000000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="10">
+        <v>0.4</v>
+      </c>
+      <c r="B41" s="1">
+        <f t="shared" si="1"/>
+        <v>2.83</v>
+      </c>
+      <c r="C41" s="13">
+        <f>AVERAGE(11006,10724,10758,10409,11260,11250,10916)</f>
+        <v>10903.285714285714</v>
+      </c>
+      <c r="D41" s="1">
+        <f t="shared" ref="D41" si="7">B41*1000/400</f>
+        <v>7.0750000000000002</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="B42" s="1">
+        <f t="shared" si="1"/>
+        <v>3.33</v>
+      </c>
+      <c r="C42" s="13">
+        <f>AVERAGE(9191,9493,9938,9394,9418,9403)</f>
+        <v>9472.8333333333339</v>
+      </c>
+      <c r="D42" s="1">
+        <f t="shared" ref="D42" si="8">B42*1000/400</f>
+        <v>8.3249999999999993</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="10">
+        <v>0.6</v>
+      </c>
+      <c r="B43" s="1">
+        <f t="shared" si="1"/>
+        <v>3.93</v>
+      </c>
+      <c r="C43" s="13">
+        <f>AVERAGE(8025,7850,8143,7780,8425,8034,7912)</f>
+        <v>8024.1428571428569</v>
+      </c>
+      <c r="D43" s="1">
+        <f t="shared" ref="D43" si="9">B43*1000/400</f>
+        <v>9.8249999999999993</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="B44" s="1">
+        <f t="shared" si="1"/>
+        <v>4.63</v>
+      </c>
+      <c r="C44" s="13">
+        <f>AVERAGE(6509,6301,6420,7031,6216,6033,6214)</f>
+        <v>6389.1428571428569</v>
+      </c>
+      <c r="D44" s="1">
+        <f t="shared" ref="D44" si="10">B44*1000/400</f>
+        <v>11.574999999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="10">
+        <v>0.8</v>
+      </c>
+      <c r="B45" s="1">
+        <f t="shared" si="1"/>
+        <v>5.43</v>
+      </c>
+      <c r="C45" s="13">
+        <f>AVERAGE(5178,5240,5275,5044,5557,5292,5022)</f>
+        <v>5229.7142857142853</v>
+      </c>
+      <c r="D45" s="1">
+        <f t="shared" ref="D45" si="11">B45*1000/400</f>
+        <v>13.574999999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="10">
+        <v>0.9</v>
+      </c>
+      <c r="B46" s="1">
+        <f t="shared" si="1"/>
+        <v>6.33</v>
+      </c>
+      <c r="C46" s="13">
+        <f>AVERAGE(4100,4050,4097,4023,4004,3902,3921)</f>
+        <v>4013.8571428571427</v>
+      </c>
+      <c r="D46" s="1">
+        <f t="shared" ref="D46" si="12">B46*1000/400</f>
+        <v>15.824999999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="10">
+        <v>1</v>
+      </c>
+      <c r="B47" s="1">
+        <f t="shared" si="1"/>
+        <v>7.33</v>
+      </c>
+      <c r="C47" s="13">
+        <f>AVERAGE(3127,3177,3173,3195,3092,3207,3216)</f>
+        <v>3169.5714285714284</v>
+      </c>
+      <c r="D47" s="1">
+        <f t="shared" ref="D47" si="13">B47*1000/400</f>
+        <v>18.324999999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="B48" s="1">
+        <f t="shared" si="1"/>
+        <v>8.83</v>
+      </c>
+      <c r="C48" s="13">
+        <f>AVERAGE(2309,2338,2262,2338,2272,2245,2220)</f>
+        <v>2283.4285714285716</v>
+      </c>
+      <c r="D48" s="1">
+        <f t="shared" ref="D48" si="14">B48*1000/400</f>
+        <v>22.074999999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="10">
+        <v>2</v>
+      </c>
+      <c r="B49" s="1">
+        <f t="shared" si="1"/>
+        <v>10.83</v>
+      </c>
+      <c r="C49" s="13">
+        <f>AVERAGE(1667,1642,1594,1715,1746,1658,1678)</f>
+        <v>1671.4285714285713</v>
+      </c>
+      <c r="D49" s="1">
+        <f t="shared" ref="D49" si="15">B49*1000/400</f>
+        <v>27.074999999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="10">
+        <v>3</v>
+      </c>
+      <c r="B50" s="1">
+        <f t="shared" si="1"/>
+        <v>13.83</v>
+      </c>
+      <c r="C50" s="13">
+        <f>AVERAGE(1173,1108,1154,1201,1133)</f>
+        <v>1153.8</v>
+      </c>
+      <c r="D50" s="1">
+        <f t="shared" ref="D50" si="16">B50*1000/400</f>
+        <v>34.575000000000003</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="10">
+        <v>5</v>
+      </c>
+      <c r="B51" s="1">
+        <f t="shared" si="1"/>
+        <v>18.829999999999998</v>
+      </c>
+      <c r="C51" s="13">
+        <f>AVERAGE(771,772,782,794,779,760,780,782)</f>
+        <v>777.5</v>
+      </c>
+      <c r="D51" s="1">
+        <f t="shared" ref="D51" si="17">B51*1000/400</f>
+        <v>47.075000000000003</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B52" s="1">
+        <f>G2-B51</f>
+        <v>6.8700000000000472</v>
       </c>
     </row>
   </sheetData>
@@ -4607,12 +5274,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="C10:C12"/>
     <mergeCell ref="B22:B24"/>
     <mergeCell ref="C22:C24"/>
     <mergeCell ref="B13:B15"/>
@@ -4621,6 +5282,12 @@
     <mergeCell ref="C16:C18"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="C19:C21"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="C10:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4628,12 +5295,204 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="F2:V21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="6:22" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="I3" s="31" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="6:22" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="I4" s="31" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" t="s">
+        <v>27</v>
+      </c>
+      <c r="T8" s="29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>1E-3</v>
+      </c>
+      <c r="G9">
+        <v>4.7</v>
+      </c>
+      <c r="H9">
+        <v>3.65</v>
+      </c>
+      <c r="T9" s="29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>250</v>
+      </c>
+      <c r="G10">
+        <v>4.38</v>
+      </c>
+      <c r="H10">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="11" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <v>500</v>
+      </c>
+      <c r="G11">
+        <v>4</v>
+      </c>
+      <c r="H11">
+        <v>2.85</v>
+      </c>
+      <c r="T11" s="30">
+        <v>9.9999999999999994E-12</v>
+      </c>
+      <c r="U11" s="30">
+        <v>-1E-10</v>
+      </c>
+      <c r="V11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <v>750</v>
+      </c>
+      <c r="G12">
+        <v>3.68</v>
+      </c>
+      <c r="H12">
+        <v>2.6</v>
+      </c>
+      <c r="T12" s="30">
+        <v>1.9999999999999999E-7</v>
+      </c>
+      <c r="U12" s="30">
+        <v>7.9999999999999996E-7</v>
+      </c>
+      <c r="V12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <v>1000</v>
+      </c>
+      <c r="G13">
+        <v>3.4</v>
+      </c>
+      <c r="H13">
+        <v>2.35</v>
+      </c>
+      <c r="T13">
+        <v>-1.6000000000000001E-3</v>
+      </c>
+      <c r="U13">
+        <v>-1.9E-3</v>
+      </c>
+      <c r="V13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <v>1250</v>
+      </c>
+      <c r="G14">
+        <v>3.2</v>
+      </c>
+      <c r="H14">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="T14">
+        <v>4.7176</v>
+      </c>
+      <c r="U14">
+        <v>3.6454</v>
+      </c>
+    </row>
+    <row r="15" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <v>1500</v>
+      </c>
+      <c r="G15">
+        <v>3</v>
+      </c>
+      <c r="H15">
+        <v>2.0499999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="6:22" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>1750</v>
+      </c>
+      <c r="G16">
+        <v>2.82</v>
+      </c>
+      <c r="H16">
+        <v>1.92</v>
+      </c>
+    </row>
+    <row r="17" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>2000</v>
+      </c>
+      <c r="G17">
+        <v>2.7</v>
+      </c>
+      <c r="H17">
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="20" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <f>G9-G17</f>
+        <v>2</v>
+      </c>
+      <c r="H20">
+        <f>H9-H17</f>
+        <v>1.8399999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <f>1.3+1.3*0.4</f>
+        <v>1.82</v>
+      </c>
+      <c r="H21">
+        <f>1.3+1.3*0.4</f>
+        <v>1.82</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>